<commit_message>
modified data files for new obj
</commit_message>
<xml_diff>
--- a/benchmarks/results/plots/results-Fairness.xlsx
+++ b/benchmarks/results/plots/results-Fairness.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,16 @@
           <t>reward</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>economic_losses</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>total_loss</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -515,6 +525,12 @@
       <c r="J2" t="n">
         <v>0</v>
       </c>
+      <c r="K2" t="n">
+        <v>98.01884882001667</v>
+      </c>
+      <c r="L2" t="n">
+        <v>98.01884882001667</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -547,7 +563,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J3" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K3" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L3" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="4">
@@ -581,7 +603,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J4" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K4" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L4" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="5">
@@ -615,7 +643,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J5" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K5" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L5" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="6">
@@ -649,7 +683,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J6" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K6" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L6" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="7">
@@ -683,7 +723,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J7" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K7" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L7" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="8">
@@ -717,7 +763,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J8" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K8" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L8" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="9">
@@ -751,7 +803,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J9" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K9" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L9" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="10">
@@ -785,7 +843,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J10" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K10" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L10" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="11">
@@ -819,7 +883,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J11" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K11" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L11" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="12">
@@ -853,7 +923,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J12" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K12" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L12" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="13">
@@ -887,7 +963,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J13" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K13" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L13" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="14">
@@ -921,7 +1003,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J14" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K14" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L14" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="15">
@@ -955,7 +1043,13 @@
         <v>10429.00587599524</v>
       </c>
       <c r="J15" t="n">
-        <v>55703198257.36978</v>
+        <v>55.70319825736978</v>
+      </c>
+      <c r="K15" t="n">
+        <v>42.31565056264689</v>
+      </c>
+      <c r="L15" t="n">
+        <v>42.31565056264689</v>
       </c>
     </row>
     <row r="16">
@@ -989,7 +1083,13 @@
         <v>4231.112192640483</v>
       </c>
       <c r="J16" t="n">
-        <v>54181032831.77833</v>
+        <v>54.18103283177832</v>
+      </c>
+      <c r="K16" t="n">
+        <v>42.26388329436435</v>
+      </c>
+      <c r="L16" t="n">
+        <v>43.83781598823835</v>
       </c>
     </row>
     <row r="17">
@@ -1023,7 +1123,13 @@
         <v>3296.43384245348</v>
       </c>
       <c r="J17" t="n">
-        <v>54653146022.72955</v>
+        <v>54.65314602272955</v>
+      </c>
+      <c r="K17" t="n">
+        <v>42.1394613833027</v>
+      </c>
+      <c r="L17" t="n">
+        <v>43.36570279728712</v>
       </c>
     </row>
     <row r="18">
@@ -1057,7 +1163,13 @@
         <v>4033.174095741991</v>
       </c>
       <c r="J18" t="n">
-        <v>54279170837.7467</v>
+        <v>54.2791708377467</v>
+      </c>
+      <c r="K18" t="n">
+        <v>42.23937634044267</v>
+      </c>
+      <c r="L18" t="n">
+        <v>43.73967798226998</v>
       </c>
     </row>
     <row r="19">
@@ -1091,7 +1203,13 @@
         <v>3745.593004266454</v>
       </c>
       <c r="J19" t="n">
-        <v>54442184115.44126</v>
+        <v>54.44218411544126</v>
+      </c>
+      <c r="K19" t="n">
+        <v>42.18334043924043</v>
+      </c>
+      <c r="L19" t="n">
+        <v>43.57666470457541</v>
       </c>
     </row>
     <row r="20">
@@ -1125,7 +1243,13 @@
         <v>4256.759957252437</v>
       </c>
       <c r="J20" t="n">
-        <v>54156038080.66071</v>
+        <v>54.15603808066071</v>
+      </c>
+      <c r="K20" t="n">
+        <v>42.27933732582964</v>
+      </c>
+      <c r="L20" t="n">
+        <v>43.86281073935596</v>
       </c>
     </row>
     <row r="21">
@@ -1159,7 +1283,13 @@
         <v>4088.130250356943</v>
       </c>
       <c r="J21" t="n">
-        <v>54252918239.13898</v>
+        <v>54.25291823913898</v>
+      </c>
+      <c r="K21" t="n">
+        <v>42.24518578260834</v>
+      </c>
+      <c r="L21" t="n">
+        <v>43.7659305808777</v>
       </c>
     </row>
     <row r="22">
@@ -1193,7 +1323,13 @@
         <v>3916.75738124368</v>
       </c>
       <c r="J22" t="n">
-        <v>54334499534.5559</v>
+        <v>54.3344995345559</v>
+      </c>
+      <c r="K22" t="n">
+        <v>42.22735353218471</v>
+      </c>
+      <c r="L22" t="n">
+        <v>43.68434928546078</v>
       </c>
     </row>
     <row r="23">
@@ -1227,7 +1363,13 @@
         <v>3415.63776739638</v>
       </c>
       <c r="J23" t="n">
-        <v>54595478717.57277</v>
+        <v>54.59547871757277</v>
+      </c>
+      <c r="K23" t="n">
+        <v>42.15278598465879</v>
+      </c>
+      <c r="L23" t="n">
+        <v>43.42337010244391</v>
       </c>
     </row>
     <row r="24">
@@ -1261,7 +1403,13 @@
         <v>3668.301783125372</v>
       </c>
       <c r="J24" t="n">
-        <v>54504389334.82131</v>
+        <v>54.50438933482131</v>
+      </c>
+      <c r="K24" t="n">
+        <v>42.14988680440002</v>
+      </c>
+      <c r="L24" t="n">
+        <v>43.51445948519537</v>
       </c>
     </row>
     <row r="25">
@@ -1295,7 +1443,13 @@
         <v>2635.781014973123</v>
       </c>
       <c r="J25" t="n">
-        <v>54977931713.78946</v>
+        <v>54.97793171378946</v>
+      </c>
+      <c r="K25" t="n">
+        <v>42.06043213573306</v>
+      </c>
+      <c r="L25" t="n">
+        <v>43.04091710622722</v>
       </c>
     </row>
     <row r="26">
@@ -1329,7 +1483,13 @@
         <v>2635.781014973123</v>
       </c>
       <c r="J26" t="n">
-        <v>54977931713.78946</v>
+        <v>54.97793171378946</v>
+      </c>
+      <c r="K26" t="n">
+        <v>42.06043213573306</v>
+      </c>
+      <c r="L26" t="n">
+        <v>43.04091710622722</v>
       </c>
     </row>
     <row r="27">
@@ -1363,7 +1523,13 @@
         <v>4140.834656601058</v>
       </c>
       <c r="J27" t="n">
-        <v>54227637385.23792</v>
+        <v>54.22763738523792</v>
+      </c>
+      <c r="K27" t="n">
+        <v>42.25086110861932</v>
+      </c>
+      <c r="L27" t="n">
+        <v>43.79121143477876</v>
       </c>
     </row>
     <row r="28">
@@ -1397,7 +1563,13 @@
         <v>3791.265742223235</v>
       </c>
       <c r="J28" t="n">
-        <v>54393790522.82607</v>
+        <v>54.39379052282607</v>
+      </c>
+      <c r="K28" t="n">
+        <v>42.21474421636126</v>
+      </c>
+      <c r="L28" t="n">
+        <v>43.62505829719061</v>
       </c>
     </row>
     <row r="29">
@@ -1431,7 +1603,13 @@
         <v>1724.2829924064</v>
       </c>
       <c r="J29" t="n">
-        <v>53259834199.56586</v>
+        <v>53.25983419956586</v>
+      </c>
+      <c r="K29" t="n">
+        <v>43.15547325137542</v>
+      </c>
+      <c r="L29" t="n">
+        <v>44.75901462045082</v>
       </c>
     </row>
     <row r="30">
@@ -1465,7 +1643,13 @@
         <v>1870.572220826859</v>
       </c>
       <c r="J30" t="n">
-        <v>52672485483.69619</v>
+        <v>52.67248548369619</v>
+      </c>
+      <c r="K30" t="n">
+        <v>43.60677653232785</v>
+      </c>
+      <c r="L30" t="n">
+        <v>45.34636333632049</v>
       </c>
     </row>
     <row r="31">
@@ -1499,7 +1683,13 @@
         <v>1882.665415555791</v>
       </c>
       <c r="J31" t="n">
-        <v>52051100212.17882</v>
+        <v>52.05110021217882</v>
+      </c>
+      <c r="K31" t="n">
+        <v>44.2169154260073</v>
+      </c>
+      <c r="L31" t="n">
+        <v>45.96774860783786</v>
       </c>
     </row>
     <row r="32">
@@ -1533,7 +1723,13 @@
         <v>1862.519036637674</v>
       </c>
       <c r="J32" t="n">
-        <v>52899639130.36214</v>
+        <v>52.89963913036214</v>
+      </c>
+      <c r="K32" t="n">
+        <v>43.38711215166814</v>
+      </c>
+      <c r="L32" t="n">
+        <v>45.11920968965454</v>
       </c>
     </row>
     <row r="33">
@@ -1567,7 +1763,13 @@
         <v>2182.839576253928</v>
       </c>
       <c r="J33" t="n">
-        <v>51226664476.70406</v>
+        <v>51.22666447670407</v>
+      </c>
+      <c r="K33" t="n">
+        <v>44.76219647125619</v>
+      </c>
+      <c r="L33" t="n">
+        <v>46.79218434331261</v>
       </c>
     </row>
     <row r="34">
@@ -1601,7 +1803,13 @@
         <v>1910.155597753896</v>
       </c>
       <c r="J34" t="n">
-        <v>51583374548.51122</v>
+        <v>51.58337454851122</v>
+      </c>
+      <c r="K34" t="n">
+        <v>44.65907588686757</v>
+      </c>
+      <c r="L34" t="n">
+        <v>46.43547427150546</v>
       </c>
     </row>
     <row r="35">
@@ -1635,7 +1843,13 @@
         <v>1916.87867845897</v>
       </c>
       <c r="J35" t="n">
-        <v>51674199740.19302</v>
+        <v>51.67419974019302</v>
+      </c>
+      <c r="K35" t="n">
+        <v>44.56199839316476</v>
+      </c>
+      <c r="L35" t="n">
+        <v>46.34464907982365</v>
       </c>
     </row>
     <row r="36">
@@ -1669,7 +1883,13 @@
         <v>2610.436284710506</v>
       </c>
       <c r="J36" t="n">
-        <v>50870414240.58946</v>
+        <v>50.87041424058946</v>
+      </c>
+      <c r="K36" t="n">
+        <v>44.72079213772634</v>
+      </c>
+      <c r="L36" t="n">
+        <v>47.14843457942722</v>
       </c>
     </row>
     <row r="37">
@@ -1703,7 +1923,13 @@
         <v>1863.679328655975</v>
       </c>
       <c r="J37" t="n">
-        <v>52460368756.39086</v>
+        <v>52.46036875639086</v>
+      </c>
+      <c r="K37" t="n">
+        <v>43.82530348219947</v>
+      </c>
+      <c r="L37" t="n">
+        <v>45.55848006362582</v>
       </c>
     </row>
     <row r="38">
@@ -1737,7 +1963,13 @@
         <v>3834.983397309869</v>
       </c>
       <c r="J38" t="n">
-        <v>52044643039.84525</v>
+        <v>52.04464303984525</v>
+      </c>
+      <c r="K38" t="n">
+        <v>42.40776421902063</v>
+      </c>
+      <c r="L38" t="n">
+        <v>45.97420578017142</v>
       </c>
     </row>
     <row r="39">
@@ -1771,7 +2003,13 @@
         <v>1926.166212183026</v>
       </c>
       <c r="J39" t="n">
-        <v>51860026680.40393</v>
+        <v>51.86002668040393</v>
+      </c>
+      <c r="K39" t="n">
+        <v>44.36753427181317</v>
+      </c>
+      <c r="L39" t="n">
+        <v>46.15882213961275</v>
       </c>
     </row>
     <row r="40">
@@ -1805,7 +2043,13 @@
         <v>1724.2829924064</v>
       </c>
       <c r="J40" t="n">
-        <v>53259834199.56586</v>
+        <v>53.25983419956586</v>
+      </c>
+      <c r="K40" t="n">
+        <v>43.15547325137542</v>
+      </c>
+      <c r="L40" t="n">
+        <v>44.75901462045082</v>
       </c>
     </row>
     <row r="41">
@@ -1839,7 +2083,13 @@
         <v>1877.907898679197</v>
       </c>
       <c r="J41" t="n">
-        <v>52250998599.83963</v>
+        <v>52.25099859983963</v>
+      </c>
+      <c r="K41" t="n">
+        <v>44.02144141367193</v>
+      </c>
+      <c r="L41" t="n">
+        <v>45.76785022017705</v>
       </c>
     </row>
     <row r="42">
@@ -1873,7 +2123,13 @@
         <v>1564.830411011497</v>
       </c>
       <c r="J42" t="n">
-        <v>49908410114.83423</v>
+        <v>49.90841011483423</v>
+      </c>
+      <c r="K42" t="n">
+        <v>45.19993003497599</v>
+      </c>
+      <c r="L42" t="n">
+        <v>48.11043870518245</v>
       </c>
     </row>
     <row r="43">
@@ -1907,7 +2163,13 @@
         <v>1768.883571723392</v>
       </c>
       <c r="J43" t="n">
-        <v>50536441643.08379</v>
+        <v>50.53644164308379</v>
+      </c>
+      <c r="K43" t="n">
+        <v>44.1923695243806</v>
+      </c>
+      <c r="L43" t="n">
+        <v>47.48240717693287</v>
       </c>
     </row>
     <row r="44">
@@ -1941,7 +2203,13 @@
         <v>1465.793544192139</v>
       </c>
       <c r="J44" t="n">
-        <v>49660854679.7615</v>
+        <v>49.6608546797615</v>
+      </c>
+      <c r="K44" t="n">
+        <v>45.63168923904469</v>
+      </c>
+      <c r="L44" t="n">
+        <v>48.35799414025518</v>
       </c>
     </row>
     <row r="45">
@@ -1975,7 +2243,13 @@
         <v>1292.247553215796</v>
       </c>
       <c r="J45" t="n">
-        <v>51440893542.48672</v>
+        <v>51.44089354248672</v>
+      </c>
+      <c r="K45" t="n">
+        <v>44.1744375025549</v>
+      </c>
+      <c r="L45" t="n">
+        <v>46.57795527752996</v>
       </c>
     </row>
     <row r="46">
@@ -2009,7 +2283,13 @@
         <v>1592.893529397573</v>
       </c>
       <c r="J46" t="n">
-        <v>50036604725.35678</v>
+        <v>50.03660472535678</v>
+      </c>
+      <c r="K46" t="n">
+        <v>45.01953938531658</v>
+      </c>
+      <c r="L46" t="n">
+        <v>47.9822440946599</v>
       </c>
     </row>
     <row r="47">
@@ -2043,7 +2323,13 @@
         <v>1556.95247103731</v>
       </c>
       <c r="J47" t="n">
-        <v>50928048746.06259</v>
+        <v>50.92804874606259</v>
+      </c>
+      <c r="K47" t="n">
+        <v>44.19494399001952</v>
+      </c>
+      <c r="L47" t="n">
+        <v>47.09080007395409</v>
       </c>
     </row>
     <row r="48">
@@ -2077,7 +2363,13 @@
         <v>1447.392551858126</v>
       </c>
       <c r="J48" t="n">
-        <v>49704590182.02235</v>
+        <v>49.70459018202234</v>
+      </c>
+      <c r="K48" t="n">
+        <v>45.62217869007696</v>
+      </c>
+      <c r="L48" t="n">
+        <v>48.31425863799433</v>
       </c>
     </row>
     <row r="49">
@@ -2111,7 +2403,13 @@
         <v>1422.344750173092</v>
       </c>
       <c r="J49" t="n">
-        <v>49633519917.82667</v>
+        <v>49.63351991782667</v>
+      </c>
+      <c r="K49" t="n">
+        <v>45.73983665058844</v>
+      </c>
+      <c r="L49" t="n">
+        <v>48.38532890219001</v>
       </c>
     </row>
     <row r="50">
@@ -2145,7 +2443,13 @@
         <v>1611.830447028359</v>
       </c>
       <c r="J50" t="n">
-        <v>50158707859.8961</v>
+        <v>50.1587078598961</v>
+      </c>
+      <c r="K50" t="n">
+        <v>44.86221450242451</v>
+      </c>
+      <c r="L50" t="n">
+        <v>47.86014096012057</v>
       </c>
     </row>
     <row r="51">
@@ -2179,7 +2483,13 @@
         <v>1575.898431722074</v>
       </c>
       <c r="J51" t="n">
-        <v>49916006815.49107</v>
+        <v>49.91600681549107</v>
+      </c>
+      <c r="K51" t="n">
+        <v>45.17174735259648</v>
+      </c>
+      <c r="L51" t="n">
+        <v>48.1028420045256</v>
       </c>
     </row>
     <row r="52">
@@ -2213,7 +2523,13 @@
         <v>1292.247553215796</v>
       </c>
       <c r="J52" t="n">
-        <v>51440893542.48672</v>
+        <v>51.44089354248672</v>
+      </c>
+      <c r="K52" t="n">
+        <v>44.1744375025549</v>
+      </c>
+      <c r="L52" t="n">
+        <v>46.57795527752996</v>
       </c>
     </row>
     <row r="53">
@@ -2247,7 +2563,13 @@
         <v>1612.672626701761</v>
       </c>
       <c r="J53" t="n">
-        <v>50418812986.83839</v>
+        <v>50.41881298683839</v>
+      </c>
+      <c r="K53" t="n">
+        <v>44.6005429621354</v>
+      </c>
+      <c r="L53" t="n">
+        <v>47.60003583317829</v>
       </c>
     </row>
     <row r="54">
@@ -2281,7 +2603,13 @@
         <v>1435.194703396241</v>
       </c>
       <c r="J54" t="n">
-        <v>49726986687.77207</v>
+        <v>49.72698668777207</v>
+      </c>
+      <c r="K54" t="n">
+        <v>45.62246959087071</v>
+      </c>
+      <c r="L54" t="n">
+        <v>48.29186213224462</v>
       </c>
     </row>
     <row r="55">
@@ -2315,7 +2643,13 @@
         <v>1200.846446841735</v>
       </c>
       <c r="J55" t="n">
-        <v>47498645451.23843</v>
+        <v>47.49864545123842</v>
+      </c>
+      <c r="K55" t="n">
+        <v>46.05317106863232</v>
+      </c>
+      <c r="L55" t="n">
+        <v>50.52020336877825</v>
       </c>
     </row>
     <row r="56">
@@ -2349,7 +2683,13 @@
         <v>1188.546264435768</v>
       </c>
       <c r="J56" t="n">
-        <v>47550731303.81823</v>
+        <v>47.55073130381823</v>
+      </c>
+      <c r="K56" t="n">
+        <v>46.04684070148503</v>
+      </c>
+      <c r="L56" t="n">
+        <v>50.46811751619845</v>
       </c>
     </row>
     <row r="57">
@@ -2383,7 +2723,13 @@
         <v>1145.00170391402</v>
       </c>
       <c r="J57" t="n">
-        <v>48300836842.26291</v>
+        <v>48.30083684226291</v>
+      </c>
+      <c r="K57" t="n">
+        <v>45.45871670435888</v>
+      </c>
+      <c r="L57" t="n">
+        <v>49.71801197775377</v>
       </c>
     </row>
     <row r="58">
@@ -2417,7 +2763,13 @@
         <v>1217.846712482625</v>
       </c>
       <c r="J58" t="n">
-        <v>47426025114.5131</v>
+        <v>47.4260251145131</v>
+      </c>
+      <c r="K58" t="n">
+        <v>46.06255206619931</v>
+      </c>
+      <c r="L58" t="n">
+        <v>50.59282370550358</v>
       </c>
     </row>
     <row r="59">
@@ -2451,7 +2803,13 @@
         <v>1192.84340711663</v>
       </c>
       <c r="J59" t="n">
-        <v>47637758681.47027</v>
+        <v>47.63775868147027</v>
+      </c>
+      <c r="K59" t="n">
+        <v>45.94382836988303</v>
+      </c>
+      <c r="L59" t="n">
+        <v>50.38109013854641</v>
       </c>
     </row>
     <row r="60">
@@ -2485,7 +2843,13 @@
         <v>1217.562341220238</v>
       </c>
       <c r="J60" t="n">
-        <v>47702276815.07964</v>
+        <v>47.70227681507964</v>
+      </c>
+      <c r="K60" t="n">
+        <v>45.78735819914484</v>
+      </c>
+      <c r="L60" t="n">
+        <v>50.31657200493703</v>
       </c>
     </row>
     <row r="61">
@@ -2519,7 +2883,13 @@
         <v>1226.563494565098</v>
       </c>
       <c r="J61" t="n">
-        <v>47406023420.66193</v>
+        <v>47.40602342066192</v>
+      </c>
+      <c r="K61" t="n">
+        <v>46.05012817623154</v>
+      </c>
+      <c r="L61" t="n">
+        <v>50.61282539935475</v>
       </c>
     </row>
     <row r="62">
@@ -2553,7 +2923,13 @@
         <v>1188.01597290274</v>
       </c>
       <c r="J62" t="n">
-        <v>47579374033.20068</v>
+        <v>47.57937403320069</v>
+      </c>
+      <c r="K62" t="n">
+        <v>46.02017060516717</v>
+      </c>
+      <c r="L62" t="n">
+        <v>50.43947478681599</v>
       </c>
     </row>
     <row r="63">
@@ -2587,7 +2963,13 @@
         <v>1242.509270239444</v>
       </c>
       <c r="J63" t="n">
-        <v>47313498031.78252</v>
+        <v>47.31349803178252</v>
+      </c>
+      <c r="K63" t="n">
+        <v>46.08333682634265</v>
+      </c>
+      <c r="L63" t="n">
+        <v>50.70535078823416</v>
       </c>
     </row>
     <row r="64">
@@ -2621,7 +3003,13 @@
         <v>1212.893732509668</v>
       </c>
       <c r="J64" t="n">
-        <v>47452807031.38995</v>
+        <v>47.45280703138995</v>
+      </c>
+      <c r="K64" t="n">
+        <v>46.05419475438281</v>
+      </c>
+      <c r="L64" t="n">
+        <v>50.56604178862672</v>
       </c>
     </row>
     <row r="65">
@@ -2655,7 +3043,13 @@
         <v>1145.00170391402</v>
       </c>
       <c r="J65" t="n">
-        <v>48300836842.26291</v>
+        <v>48.30083684226291</v>
+      </c>
+      <c r="K65" t="n">
+        <v>45.45871670435888</v>
+      </c>
+      <c r="L65" t="n">
+        <v>49.71801197775377</v>
       </c>
     </row>
     <row r="66">
@@ -2689,7 +3083,13 @@
         <v>1211.512997841839</v>
       </c>
       <c r="J66" t="n">
-        <v>47812253736.98629</v>
+        <v>47.81225373698629</v>
+      </c>
+      <c r="K66" t="n">
+        <v>45.69988424781952</v>
+      </c>
+      <c r="L66" t="n">
+        <v>50.20659508303039</v>
       </c>
     </row>
     <row r="67">
@@ -2723,7 +3123,13 @@
         <v>1233.950454000473</v>
       </c>
       <c r="J67" t="n">
-        <v>47356757301.9763</v>
+        <v>47.3567573019763</v>
+      </c>
+      <c r="K67" t="n">
+        <v>46.07191552235265</v>
+      </c>
+      <c r="L67" t="n">
+        <v>50.66209151804037</v>
       </c>
     </row>
     <row r="68">
@@ -2757,7 +3163,13 @@
         <v>1040.650553557806</v>
       </c>
       <c r="J68" t="n">
-        <v>44331463352.80103</v>
+        <v>44.33146335280103</v>
+      </c>
+      <c r="K68" t="n">
+        <v>47.88070679301862</v>
+      </c>
+      <c r="L68" t="n">
+        <v>53.68738546721563</v>
       </c>
     </row>
     <row r="69">
@@ -2791,7 +3203,13 @@
         <v>1072.623419102717</v>
       </c>
       <c r="J69" t="n">
-        <v>44022153825.59327</v>
+        <v>44.02215382559327</v>
+      </c>
+      <c r="K69" t="n">
+        <v>48.01161238253772</v>
+      </c>
+      <c r="L69" t="n">
+        <v>53.99669499442341</v>
       </c>
     </row>
     <row r="70">
@@ -2825,7 +3243,13 @@
         <v>1346.519853261003</v>
       </c>
       <c r="J70" t="n">
-        <v>44533667243.35636</v>
+        <v>44.53366724335636</v>
+      </c>
+      <c r="K70" t="n">
+        <v>45.97179671410257</v>
+      </c>
+      <c r="L70" t="n">
+        <v>53.48518157666032</v>
       </c>
     </row>
     <row r="71">
@@ -2859,7 +3283,13 @@
         <v>1325.868614069322</v>
       </c>
       <c r="J71" t="n">
-        <v>43796183409.53561</v>
+        <v>43.79618340953561</v>
+      </c>
+      <c r="K71" t="n">
+        <v>46.82451145785758</v>
+      </c>
+      <c r="L71" t="n">
+        <v>54.22266541048107</v>
       </c>
     </row>
     <row r="72">
@@ -2893,7 +3323,13 @@
         <v>1276.002434247798</v>
       </c>
       <c r="J72" t="n">
-        <v>43781293425.51886</v>
+        <v>43.78129342551886</v>
+      </c>
+      <c r="K72" t="n">
+        <v>47.11764746974928</v>
+      </c>
+      <c r="L72" t="n">
+        <v>54.23755539449782</v>
       </c>
     </row>
     <row r="73">
@@ -2927,7 +3363,13 @@
         <v>1040.049997822283</v>
       </c>
       <c r="J73" t="n">
-        <v>44583235621.82331</v>
+        <v>44.58323562182331</v>
+      </c>
+      <c r="K73" t="n">
+        <v>47.63228553761971</v>
+      </c>
+      <c r="L73" t="n">
+        <v>53.43561319819337</v>
       </c>
     </row>
     <row r="74">
@@ -2961,7 +3403,13 @@
         <v>1007.580978298291</v>
       </c>
       <c r="J74" t="n">
-        <v>44962726484.19868</v>
+        <v>44.96272648419868</v>
+      </c>
+      <c r="K74" t="n">
+        <v>47.43396707994586</v>
+      </c>
+      <c r="L74" t="n">
+        <v>53.056122335818</v>
       </c>
     </row>
     <row r="75">
@@ -2995,7 +3443,13 @@
         <v>1026.894680823912</v>
       </c>
       <c r="J75" t="n">
-        <v>44734433090.45485</v>
+        <v>44.73443309045485</v>
+      </c>
+      <c r="K75" t="n">
+        <v>47.55449282374046</v>
+      </c>
+      <c r="L75" t="n">
+        <v>53.28441572956183</v>
       </c>
     </row>
     <row r="76">
@@ -3029,7 +3483,13 @@
         <v>1007.580978298291</v>
       </c>
       <c r="J76" t="n">
-        <v>44962726484.19868</v>
+        <v>44.96272648419868</v>
+      </c>
+      <c r="K76" t="n">
+        <v>47.43396707994586</v>
+      </c>
+      <c r="L76" t="n">
+        <v>53.056122335818</v>
       </c>
     </row>
     <row r="77">
@@ -3063,7 +3523,13 @@
         <v>1298.570228359109</v>
       </c>
       <c r="J77" t="n">
-        <v>43848668432.66286</v>
+        <v>43.84866843266285</v>
+      </c>
+      <c r="K77" t="n">
+        <v>46.92434745507822</v>
+      </c>
+      <c r="L77" t="n">
+        <v>54.17018038735382</v>
       </c>
     </row>
     <row r="78">
@@ -3097,7 +3563,13 @@
         <v>1313.483378040344</v>
       </c>
       <c r="J78" t="n">
-        <v>43679043020.31744</v>
+        <v>43.67904302031744</v>
+      </c>
+      <c r="K78" t="n">
+        <v>47.01075966206562</v>
+      </c>
+      <c r="L78" t="n">
+        <v>54.33980579969924</v>
       </c>
     </row>
     <row r="79">
@@ -3131,7 +3603,13 @@
         <v>1040.672136135463</v>
       </c>
       <c r="J79" t="n">
-        <v>44455528376.12134</v>
+        <v>44.45552837612134</v>
+      </c>
+      <c r="K79" t="n">
+        <v>47.75652134205526</v>
+      </c>
+      <c r="L79" t="n">
+        <v>53.56332044389534</v>
       </c>
     </row>
     <row r="80">
@@ -3165,7 +3643,13 @@
         <v>1040.196116688402</v>
       </c>
       <c r="J80" t="n">
-        <v>44209847205.40562</v>
+        <v>44.20984720540562</v>
+      </c>
+      <c r="K80" t="n">
+        <v>48.00485863202475</v>
+      </c>
+      <c r="L80" t="n">
+        <v>53.80900161461106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>